<commit_message>
congestion details, CWND fairness calculation
</commit_message>
<xml_diff>
--- a/ch_congestion/standalone/cwnd_fairness.xlsx
+++ b/ch_congestion/standalone/cwnd_fairness.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hkarl/compnet/lehre/lectures/rnetze/slides/ComputerNetworks/ch_congestion/standalone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E202871A-0FFF-AA47-AF96-752E1FBB8E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D6E780-E11C-9D40-AB4C-452EA5ECC1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40960" yWindow="15300" windowWidth="28040" windowHeight="17440" xr2:uid="{27441BEE-9363-ED4B-8759-6193750864A4}"/>
+    <workbookView xWindow="19440" yWindow="6840" windowWidth="28040" windowHeight="17440" xr2:uid="{27441BEE-9363-ED4B-8759-6193750864A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Ratio</t>
+  </si>
+  <si>
+    <t>1/RTT1</t>
+  </si>
+  <si>
+    <t>1/RTT2</t>
+  </si>
+  <si>
+    <t>bottleneck rate</t>
   </si>
 </sst>
 </file>
@@ -390,7 +399,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -407,19 +416,19 @@
       </c>
       <c r="D1">
         <f>$H$1-B1-C1</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1">
-        <v>2</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="G1">
         <v>1</v>
       </c>
       <c r="H1">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -428,11 +437,11 @@
       </c>
       <c r="B2">
         <f>B1+$D1*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.3333333333333339</v>
+        <v>11.0039980009995</v>
       </c>
       <c r="C2">
         <f>C1+$D1*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.666666666666667</v>
+        <v>8.9960019990004998</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D17" si="0">$H$1-B2-C2</f>
@@ -440,7 +449,16 @@
       </c>
       <c r="E2">
         <f>B2/C2</f>
-        <v>2.375</v>
+        <v>1.2232098216765734</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -449,19 +467,19 @@
       </c>
       <c r="B3">
         <f>B2/2</f>
-        <v>3.166666666666667</v>
+        <v>5.5019990004997501</v>
       </c>
       <c r="C3">
         <f>C2/2</f>
-        <v>1.3333333333333335</v>
+        <v>4.4980009995002499</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E34" si="1">B3/C3</f>
-        <v>2.375</v>
+        <v>1.2232098216765734</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -470,11 +488,11 @@
       </c>
       <c r="B4">
         <f>B3+$D3*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.166666666666667</v>
+        <v>10.504497751124436</v>
       </c>
       <c r="C4">
         <f>C3+$D3*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.8333333333333335</v>
+        <v>9.4955022488755638</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
@@ -482,7 +500,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>2.1764705882352939</v>
+        <v>1.106260361569432</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -491,19 +509,19 @@
       </c>
       <c r="B5">
         <f>B4/2</f>
-        <v>3.0833333333333335</v>
+        <v>5.2522488755622181</v>
       </c>
       <c r="C5">
         <f>C4/2</f>
-        <v>1.4166666666666667</v>
+        <v>4.7477511244377819</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>4.4999999999999991</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>2.1764705882352939</v>
+        <v>1.106260361569432</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -512,11 +530,11 @@
       </c>
       <c r="B6">
         <f t="shared" ref="B6:B17" si="2">B5+$D5*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.083333333333333</v>
+        <v>10.254747626186905</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C17" si="3">C5+$D5*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9166666666666665</v>
+        <v>9.7452523738130949</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -524,7 +542,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>2.0857142857142859</v>
+        <v>1.0522813810079354</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -533,19 +551,19 @@
       </c>
       <c r="B7">
         <f t="shared" ref="B7:B17" si="4">B6/2</f>
-        <v>3.0416666666666665</v>
+        <v>5.1273738130934525</v>
       </c>
       <c r="C7">
         <f t="shared" ref="C7:C17" si="5">C6/2</f>
-        <v>1.4583333333333333</v>
+        <v>4.8726261869065475</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>4.5000000000000009</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>2.0857142857142859</v>
+        <v>1.0522813810079354</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -554,11 +572,11 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B17" si="6">B7+$D7*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.041666666666667</v>
+        <v>10.129872563718139</v>
       </c>
       <c r="C8">
         <f t="shared" ref="C8:C17" si="7">C7+$D7*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9583333333333335</v>
+        <v>9.8701274362818605</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -566,7 +584,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>2.0422535211267605</v>
+        <v>1.0263162891374102</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -575,19 +593,19 @@
       </c>
       <c r="B9">
         <f t="shared" ref="B9:B17" si="8">B8/2</f>
-        <v>3.0208333333333335</v>
+        <v>5.0649362818590697</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:C17" si="9">C8/2</f>
-        <v>1.4791666666666667</v>
+        <v>4.9350637181409303</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>4.4999999999999991</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>2.0422535211267605</v>
+        <v>1.0263162891374102</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -596,11 +614,11 @@
       </c>
       <c r="B10">
         <f t="shared" ref="B10:B17" si="10">B9+$D9*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.020833333333333</v>
+        <v>10.067435032483758</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C17" si="11">C9+$D9*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9791666666666665</v>
+        <v>9.9325649675162424</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -608,7 +626,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>2.0209790209790208</v>
+        <v>1.013578573652284</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -617,19 +635,19 @@
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B17" si="12">B10/2</f>
-        <v>3.0104166666666665</v>
+        <v>5.0337175162418788</v>
       </c>
       <c r="C11">
         <f t="shared" ref="C11:C17" si="13">C10/2</f>
-        <v>1.4895833333333333</v>
+        <v>4.9662824837581212</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>4.5000000000000009</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>2.0209790209790208</v>
+        <v>1.013578573652284</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -638,11 +656,11 @@
       </c>
       <c r="B12">
         <f t="shared" ref="B12:B17" si="14">B11+$D11*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.010416666666667</v>
+        <v>10.036216266866566</v>
       </c>
       <c r="C12">
         <f t="shared" ref="C12:C17" si="15">C11+$D11*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9895833333333335</v>
+        <v>9.9637837331334342</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -650,7 +668,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>2.010452961672474</v>
+        <v>1.007269581082161</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -659,19 +677,19 @@
       </c>
       <c r="B13">
         <f t="shared" ref="B13:B17" si="16">B12/2</f>
-        <v>3.0052083333333335</v>
+        <v>5.0181081334332829</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13:C17" si="17">C12/2</f>
-        <v>1.4947916666666667</v>
+        <v>4.9818918665667171</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>4.4999999999999991</v>
+        <v>10</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>2.010452961672474</v>
+        <v>1.007269581082161</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -680,11 +698,11 @@
       </c>
       <c r="B14">
         <f t="shared" ref="B14:B17" si="18">B13+$D13*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.005208333333333</v>
+        <v>10.020606884057969</v>
       </c>
       <c r="C14">
         <f t="shared" ref="C14:C17" si="19">C13+$D13*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9947916666666665</v>
+        <v>9.979393115942031</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -692,7 +710,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>2.0052173913043476</v>
+        <v>1.0041298872223101</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -701,19 +719,19 @@
       </c>
       <c r="B15">
         <f t="shared" ref="B15:B17" si="20">B14/2</f>
-        <v>3.0026041666666665</v>
+        <v>5.0103034420289845</v>
       </c>
       <c r="C15">
         <f t="shared" ref="C15:C17" si="21">C14/2</f>
-        <v>1.4973958333333333</v>
+        <v>4.9896965579710155</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>4.5000000000000009</v>
+        <v>10</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>2.0052173913043476</v>
+        <v>1.0041298872223101</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -722,11 +740,11 @@
       </c>
       <c r="B16">
         <f t="shared" ref="B16:B17" si="22">B15+$D15*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.002604166666667</v>
+        <v>10.012802192653671</v>
       </c>
       <c r="C16">
         <f t="shared" ref="C16:C17" si="23">C15+$D15*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9973958333333335</v>
+        <v>9.9871978073463286</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -734,7 +752,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>2.0026064291920069</v>
+        <v>1.0025637206553082</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -743,19 +761,19 @@
       </c>
       <c r="B17">
         <f t="shared" ref="B17:C17" si="24">B16/2</f>
-        <v>3.0013020833333335</v>
+        <v>5.0064010963268357</v>
       </c>
       <c r="C17">
         <f t="shared" si="24"/>
-        <v>1.4986979166666667</v>
+        <v>4.9935989036731643</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>4.4999999999999991</v>
+        <v>10</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>2.0026064291920069</v>
+        <v>1.0025637206553082</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -764,11 +782,11 @@
       </c>
       <c r="B18">
         <f t="shared" ref="B18:B34" si="25">B17+$D17*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.001302083333333</v>
+        <v>10.008899846951522</v>
       </c>
       <c r="C18">
         <f t="shared" ref="C18:C34" si="26">C17+$D17*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9986979166666665</v>
+        <v>9.9911001530484782</v>
       </c>
       <c r="D18">
         <f t="shared" ref="D18:D34" si="27">$H$1-B18-C18</f>
@@ -776,7 +794,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>2.0013026487190619</v>
+        <v>1.0017815549469407</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -785,19 +803,19 @@
       </c>
       <c r="B19">
         <f t="shared" ref="B19:B34" si="28">B18/2</f>
-        <v>3.0006510416666665</v>
+        <v>5.0044499234757609</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:C34" si="29">C18/2</f>
-        <v>1.4993489583333333</v>
+        <v>4.9955500765242391</v>
       </c>
       <c r="D19">
         <f t="shared" si="27"/>
-        <v>4.5000000000000009</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>2.0013026487190619</v>
+        <v>1.0017815549469407</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -806,11 +824,11 @@
       </c>
       <c r="B20">
         <f t="shared" ref="B20:B34" si="30">B19+$D19*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.000651041666667</v>
+        <v>10.006948674100448</v>
       </c>
       <c r="C20">
         <f t="shared" ref="C20:C34" si="31">C19+$D19*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9993489583333335</v>
+        <v>9.9930513258995521</v>
       </c>
       <c r="D20">
         <f t="shared" si="27"/>
@@ -818,7 +836,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>2.0006511829824181</v>
+        <v>1.0013907011730119</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -827,19 +845,19 @@
       </c>
       <c r="B21">
         <f t="shared" ref="B21:B34" si="32">B20/2</f>
-        <v>3.0003255208333335</v>
+        <v>5.0034743370502239</v>
       </c>
       <c r="C21">
         <f t="shared" ref="C21:C34" si="33">C20/2</f>
-        <v>1.4996744791666667</v>
+        <v>4.9965256629497761</v>
       </c>
       <c r="D21">
         <f t="shared" si="27"/>
-        <v>4.4999999999999991</v>
+        <v>10</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>2.0006511829824181</v>
+        <v>1.0013907011730119</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -848,11 +866,11 @@
       </c>
       <c r="B22">
         <f t="shared" ref="B22:B34" si="34">B21+$D21*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.000325520833333</v>
+        <v>10.00597308767491</v>
       </c>
       <c r="C22">
         <f t="shared" ref="C22:C34" si="35">C21+$D21*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9996744791666665</v>
+        <v>9.99402691232509</v>
       </c>
       <c r="D22">
         <f t="shared" si="27"/>
@@ -860,7 +878,7 @@
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>2.0003255561584372</v>
+        <v>1.0011953315169773</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -869,19 +887,19 @@
       </c>
       <c r="B23">
         <f t="shared" ref="B23:B34" si="36">B22/2</f>
-        <v>3.0001627604166665</v>
+        <v>5.002986543837455</v>
       </c>
       <c r="C23">
         <f t="shared" ref="C23:C34" si="37">C22/2</f>
-        <v>1.4998372395833333</v>
+        <v>4.997013456162545</v>
       </c>
       <c r="D23">
         <f t="shared" si="27"/>
-        <v>4.5000000000000009</v>
+        <v>10</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>2.0003255561584372</v>
+        <v>1.0011953315169773</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -890,11 +908,11 @@
       </c>
       <c r="B24">
         <f t="shared" ref="B24:B34" si="38">B23+$D23*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.000162760416667</v>
+        <v>10.005485294462142</v>
       </c>
       <c r="C24">
         <f t="shared" ref="C24:C34" si="39">C23+$D23*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9998372395833335</v>
+        <v>9.994514705537858</v>
       </c>
       <c r="D24">
         <f t="shared" si="27"/>
@@ -902,7 +920,7 @@
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>2.0001627692474635</v>
+        <v>1.0010976609918043</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -911,19 +929,19 @@
       </c>
       <c r="B25">
         <f t="shared" ref="B25:B34" si="40">B24/2</f>
-        <v>3.0000813802083335</v>
+        <v>5.002742647231071</v>
       </c>
       <c r="C25">
         <f t="shared" ref="C25:C34" si="41">C24/2</f>
-        <v>1.4999186197916667</v>
+        <v>4.997257352768929</v>
       </c>
       <c r="D25">
         <f t="shared" si="27"/>
-        <v>4.4999999999999991</v>
+        <v>10</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>2.0001627692474635</v>
+        <v>1.0010976609918043</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -932,11 +950,11 @@
       </c>
       <c r="B26">
         <f t="shared" ref="B26:B34" si="42">B25+$D25*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.000081380208333</v>
+        <v>10.005241397855759</v>
       </c>
       <c r="C26">
         <f t="shared" ref="C26:C34" si="43">C25+$D25*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9999186197916665</v>
+        <v>9.9947586021442412</v>
       </c>
       <c r="D26">
         <f t="shared" si="27"/>
@@ -944,7 +962,7 @@
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>2.0000813824159724</v>
+        <v>1.0010488293043185</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -953,19 +971,19 @@
       </c>
       <c r="B27">
         <f t="shared" ref="B27:B34" si="44">B26/2</f>
-        <v>3.0000406901041665</v>
+        <v>5.0026206989278794</v>
       </c>
       <c r="C27">
         <f t="shared" ref="C27:C34" si="45">C26/2</f>
-        <v>1.4999593098958333</v>
+        <v>4.9973793010721206</v>
       </c>
       <c r="D27">
         <f t="shared" si="27"/>
-        <v>4.5000000000000009</v>
+        <v>10</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>2.0000813824159724</v>
+        <v>1.0010488293043185</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -974,11 +992,11 @@
       </c>
       <c r="B28">
         <f t="shared" ref="B28:B34" si="46">B27+$D27*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.000040690104167</v>
+        <v>10.005119449552566</v>
       </c>
       <c r="C28">
         <f t="shared" ref="C28:C34" si="47">C27+$D27*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9999593098958335</v>
+        <v>9.9948805504474336</v>
       </c>
       <c r="D28">
         <f t="shared" si="27"/>
@@ -986,7 +1004,7 @@
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>2.000040690656069</v>
+        <v>1.0010244143542741</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -995,19 +1013,19 @@
       </c>
       <c r="B29">
         <f t="shared" ref="B29:B34" si="48">B28/2</f>
-        <v>3.0000203450520835</v>
+        <v>5.0025597247762832</v>
       </c>
       <c r="C29">
         <f t="shared" ref="C29:C34" si="49">C28/2</f>
-        <v>1.4999796549479167</v>
+        <v>4.9974402752237168</v>
       </c>
       <c r="D29">
         <f t="shared" si="27"/>
-        <v>4.4999999999999991</v>
+        <v>10</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>2.000040690656069</v>
+        <v>1.0010244143542741</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1016,11 +1034,11 @@
       </c>
       <c r="B30">
         <f t="shared" ref="B30:B34" si="50">B29+$D29*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.000020345052083</v>
+        <v>10.00505847540097</v>
       </c>
       <c r="C30">
         <f t="shared" ref="C30:C34" si="51">C29+$D29*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9999796549479165</v>
+        <v>9.9949415245990298</v>
       </c>
       <c r="D30">
         <f t="shared" si="27"/>
@@ -1028,7 +1046,7 @@
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
-        <v>2.000020345190058</v>
+        <v>1.001012207102667</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1037,19 +1055,19 @@
       </c>
       <c r="B31">
         <f t="shared" ref="B31:B34" si="52">B30/2</f>
-        <v>3.0000101725260415</v>
+        <v>5.0025292377004851</v>
       </c>
       <c r="C31">
         <f t="shared" ref="C31:C34" si="53">C30/2</f>
-        <v>1.4999898274739583</v>
+        <v>4.9974707622995149</v>
       </c>
       <c r="D31">
         <f t="shared" si="27"/>
-        <v>4.5000000000000009</v>
+        <v>10</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
-        <v>2.000020345190058</v>
+        <v>1.001012207102667</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1058,11 +1076,11 @@
       </c>
       <c r="B32">
         <f t="shared" ref="B32:B34" si="54">B31+$D31*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.000010172526042</v>
+        <v>10.005027988325171</v>
       </c>
       <c r="C32">
         <f t="shared" ref="C32:C34" si="55">C31+$D31*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.9999898274739585</v>
+        <v>9.9949720116748288</v>
       </c>
       <c r="D32">
         <f t="shared" si="27"/>
@@ -1070,7 +1088,7 @@
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
-        <v>2.0000101725605353</v>
+        <v>1.0010061035327158</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1079,19 +1097,19 @@
       </c>
       <c r="B33">
         <f t="shared" ref="B33:B34" si="56">B32/2</f>
-        <v>3.000005086263021</v>
+        <v>5.0025139941625856</v>
       </c>
       <c r="C33">
         <f t="shared" ref="C33:C34" si="57">C32/2</f>
-        <v>1.4999949137369792</v>
+        <v>4.9974860058374144</v>
       </c>
       <c r="D33">
         <f t="shared" si="27"/>
-        <v>4.4999999999999991</v>
+        <v>10</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
-        <v>2.0000101725605353</v>
+        <v>1.0010061035327158</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1100,11 +1118,11 @@
       </c>
       <c r="B34">
         <f t="shared" ref="B34" si="58">B33+$D33*$F$1/SUM($F$1:$G$1)</f>
-        <v>6.0000050862630205</v>
+        <v>10.005012744787273</v>
       </c>
       <c r="C34">
         <f t="shared" ref="C34" si="59">C33+$D33*$G$1/SUM($F$1:$G$1)</f>
-        <v>2.999994913736979</v>
+        <v>9.9949872552127275</v>
       </c>
       <c r="D34">
         <f t="shared" si="27"/>
@@ -1112,7 +1130,7 @@
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
-        <v>2.0000050862716443</v>
+        <v>1.0010030517617035</v>
       </c>
     </row>
   </sheetData>

</xml_diff>